<commit_message>
plot with real data for inference
</commit_message>
<xml_diff>
--- a/plot/Comparison_accuracy/comparison.xlsx
+++ b/plot/Comparison_accuracy/comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuboluo/Documents/PycharmProjects/SmartSwitch/plot/Comparison_accuracy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B11DDE3C-3B0E-3E4B-B25B-91A425CF6861}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDCB37D9-DDC1-E740-BCCC-5984B8A5723C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15860" activeTab="3" xr2:uid="{A33675B7-7F4F-C34D-AB6F-57998B81D61A}"/>
   </bookViews>
@@ -235,12 +235,6 @@
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -250,6 +244,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -576,14 +576,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
@@ -719,14 +719,14 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
+      <c r="B12" s="18"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
@@ -807,24 +807,24 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
@@ -905,14 +905,14 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -937,14 +937,14 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
@@ -996,8 +996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{803D7DDF-C6E5-DB46-8AC4-11520FE3D49F}">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="125" workbookViewId="0">
-      <selection activeCell="G24" sqref="A1:XFD1048576"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1006,16 +1006,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="14" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="14">
+      <c r="F1" s="12">
         <v>5</v>
       </c>
     </row>
@@ -1178,14 +1178,14 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
@@ -1209,19 +1209,19 @@
       <c r="A13" s="5">
         <v>1</v>
       </c>
-      <c r="B13" s="13">
+      <c r="B13" s="11">
         <v>0.74</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C13" s="11">
         <v>2.57</v>
       </c>
-      <c r="D13" s="13">
+      <c r="D13" s="11">
         <v>2.57</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="11">
         <v>2.6</v>
       </c>
-      <c r="F13" s="13">
+      <c r="F13" s="11">
         <v>1.3</v>
       </c>
     </row>
@@ -1229,19 +1229,19 @@
       <c r="A14" s="5">
         <v>2</v>
       </c>
-      <c r="B14" s="13">
+      <c r="B14" s="11">
         <v>3.81</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="11">
         <v>5.25</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14" s="11">
         <v>5.25</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="11">
         <v>5.28</v>
       </c>
-      <c r="F14" s="13">
+      <c r="F14" s="11">
         <v>3.01</v>
       </c>
     </row>
@@ -1249,19 +1249,19 @@
       <c r="A15" s="5">
         <v>3</v>
       </c>
-      <c r="B15" s="13">
+      <c r="B15" s="11">
         <v>1.18</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C15" s="11">
         <v>1.85</v>
       </c>
-      <c r="D15" s="13">
+      <c r="D15" s="11">
         <v>1.85</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15" s="11">
         <v>1.86</v>
       </c>
-      <c r="F15" s="13">
+      <c r="F15" s="11">
         <v>1.4E-2</v>
       </c>
     </row>
@@ -1269,19 +1269,19 @@
       <c r="A16" s="5">
         <v>4</v>
       </c>
-      <c r="B16" s="13">
+      <c r="B16" s="11">
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="C16" s="13">
+      <c r="C16" s="11">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="D16" s="13">
+      <c r="D16" s="11">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16" s="11">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="F16" s="13">
+      <c r="F16" s="11">
         <v>1.7000000000000001E-2</v>
       </c>
     </row>
@@ -1289,19 +1289,19 @@
       <c r="A17" s="5">
         <v>5</v>
       </c>
-      <c r="B17" s="13">
+      <c r="B17" s="11">
         <v>0.05</v>
       </c>
-      <c r="C17" s="13">
+      <c r="C17" s="11">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D17" s="11">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="11">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="F17" s="13">
+      <c r="F17" s="11">
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
@@ -1309,16 +1309,16 @@
       <c r="A18" s="5">
         <v>6</v>
       </c>
-      <c r="B18" s="13">
+      <c r="B18" s="11">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="C18" s="13">
+      <c r="C18" s="11">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="D18" s="13">
+      <c r="D18" s="11">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="11">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="F18" s="6">
@@ -1351,14 +1351,14 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18"/>
+      <c r="F22" s="18"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
@@ -1404,14 +1404,14 @@
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="11" t="s">
+      <c r="A27" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
@@ -1480,12 +1480,12 @@
       <c r="A31" s="9"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="11" t="s">
+      <c r="A33" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B33" s="11"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
@@ -1502,14 +1502,14 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="11" t="s">
+      <c r="A37" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="18"/>
+      <c r="D37" s="18"/>
+      <c r="E37" s="18"/>
+      <c r="F37" s="18"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
@@ -1593,7 +1593,7 @@
   <dimension ref="A1:F66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:F21"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1602,16 +1602,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="14" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="14">
+      <c r="F1" s="12">
         <v>5</v>
       </c>
     </row>
@@ -1738,19 +1738,19 @@
         <v>18</v>
       </c>
       <c r="B7" s="7">
-        <v>30</v>
+        <v>30.26</v>
       </c>
       <c r="C7" s="7">
-        <v>30</v>
+        <v>40.58</v>
       </c>
       <c r="D7" s="7">
-        <v>30</v>
+        <v>40.58</v>
       </c>
       <c r="E7" s="7">
-        <v>30</v>
+        <v>41.06</v>
       </c>
       <c r="F7" s="7">
-        <v>30</v>
+        <v>19.72</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1758,30 +1758,30 @@
         <v>15</v>
       </c>
       <c r="B8" s="7">
-        <v>20</v>
+        <v>18.21</v>
       </c>
       <c r="C8" s="7">
-        <v>20</v>
+        <v>17.73</v>
       </c>
       <c r="D8" s="7">
-        <v>20</v>
+        <v>17.73</v>
       </c>
       <c r="E8" s="7">
-        <v>20</v>
+        <v>18.09</v>
       </c>
       <c r="F8" s="7">
-        <v>20</v>
+        <v>8.81</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
@@ -1807,19 +1807,19 @@
       <c r="A13" s="5">
         <v>1</v>
       </c>
-      <c r="B13" s="15">
+      <c r="B13" s="13">
         <v>0.74</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="13">
         <v>2.57</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="13">
         <v>2.57</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="13">
         <v>2.6</v>
       </c>
-      <c r="F13" s="15">
+      <c r="F13" s="13">
         <v>1.3</v>
       </c>
     </row>
@@ -1827,19 +1827,19 @@
       <c r="A14" s="5">
         <v>2</v>
       </c>
-      <c r="B14" s="15">
+      <c r="B14" s="13">
         <v>3.81</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="13">
         <v>5.25</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="13">
         <v>5.25</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E14" s="13">
         <v>5.28</v>
       </c>
-      <c r="F14" s="15">
+      <c r="F14" s="13">
         <v>3.01</v>
       </c>
     </row>
@@ -1847,19 +1847,19 @@
       <c r="A15" s="5">
         <v>3</v>
       </c>
-      <c r="B15" s="15">
+      <c r="B15" s="13">
         <v>1.18</v>
       </c>
-      <c r="C15" s="15">
+      <c r="C15" s="13">
         <v>1.85</v>
       </c>
-      <c r="D15" s="15">
+      <c r="D15" s="13">
         <v>1.85</v>
       </c>
-      <c r="E15" s="15">
+      <c r="E15" s="13">
         <v>1.86</v>
       </c>
-      <c r="F15" s="15">
+      <c r="F15" s="13">
         <v>1.4E-2</v>
       </c>
     </row>
@@ -1867,19 +1867,19 @@
       <c r="A16" s="5">
         <v>4</v>
       </c>
-      <c r="B16" s="15">
+      <c r="B16" s="13">
         <v>7.2999999999999995E-2</v>
       </c>
-      <c r="C16" s="15">
+      <c r="C16" s="13">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="13">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="E16" s="15">
+      <c r="E16" s="13">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="F16" s="15">
+      <c r="F16" s="13">
         <v>1.7000000000000001E-2</v>
       </c>
     </row>
@@ -1887,19 +1887,19 @@
       <c r="A17" s="5">
         <v>5</v>
       </c>
-      <c r="B17" s="15">
+      <c r="B17" s="13">
         <v>0.05</v>
       </c>
-      <c r="C17" s="15">
+      <c r="C17" s="13">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="D17" s="15">
+      <c r="D17" s="13">
         <v>4.2000000000000003E-2</v>
       </c>
-      <c r="E17" s="15">
+      <c r="E17" s="13">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="F17" s="15">
+      <c r="F17" s="13">
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
@@ -1907,19 +1907,19 @@
       <c r="A18" s="5">
         <v>6</v>
       </c>
-      <c r="B18" s="15">
+      <c r="B18" s="13">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="C18" s="15">
+      <c r="C18" s="13">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D18" s="13">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="E18" s="15">
+      <c r="E18" s="13">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="F18" s="15">
+      <c r="F18" s="13">
         <v>0</v>
       </c>
     </row>
@@ -1927,36 +1927,36 @@
       <c r="A19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="15">
+      <c r="B19" s="13">
         <f>SUM(B13:B18)</f>
         <v>5.8609999999999998</v>
       </c>
-      <c r="C19" s="15">
+      <c r="C19" s="13">
         <f t="shared" ref="C19:F19" si="0">SUM(C13:C18)</f>
         <v>9.7690000000000001</v>
       </c>
-      <c r="D19" s="15">
+      <c r="D19" s="13">
         <f t="shared" si="0"/>
         <v>9.7690000000000001</v>
       </c>
-      <c r="E19" s="15">
+      <c r="E19" s="13">
         <f t="shared" si="0"/>
         <v>9.8330000000000002</v>
       </c>
-      <c r="F19" s="15">
+      <c r="F19" s="13">
         <f t="shared" si="0"/>
         <v>4.3470000000000004</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
+      <c r="B21" s="18"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
@@ -1982,23 +1982,23 @@
       <c r="A23" s="5">
         <v>1</v>
       </c>
-      <c r="B23" s="19">
+      <c r="B23" s="17">
         <f>B50/B60*D60</f>
         <v>2.2850000000000001E-3</v>
       </c>
-      <c r="C23" s="19">
+      <c r="C23" s="17">
         <f>C50/B60*D60</f>
         <v>6.398E-3</v>
       </c>
-      <c r="D23" s="19">
+      <c r="D23" s="17">
         <f>D50/B60*D60</f>
         <v>6.398E-3</v>
       </c>
-      <c r="E23" s="19">
+      <c r="E23" s="17">
         <f>E50/B60*D60</f>
         <v>6.398E-3</v>
       </c>
-      <c r="F23" s="19">
+      <c r="F23" s="17">
         <f>F50/B60*D60</f>
         <v>7.5405000000000003E-3</v>
       </c>
@@ -2007,23 +2007,23 @@
       <c r="A24" s="5">
         <v>2</v>
       </c>
-      <c r="B24" s="19">
+      <c r="B24" s="17">
         <f>B51/B60*D60</f>
         <v>6.6265000000000004E-2</v>
       </c>
-      <c r="C24" s="19">
+      <c r="C24" s="17">
         <f>C51/B60*D60</f>
         <v>6.6265000000000004E-2</v>
       </c>
-      <c r="D24" s="19">
+      <c r="D24" s="17">
         <f>D51/B60*D60</f>
         <v>6.6265000000000004E-2</v>
       </c>
-      <c r="E24" s="19">
+      <c r="E24" s="17">
         <f>E51/B60*D60</f>
         <v>6.6265000000000004E-2</v>
       </c>
-      <c r="F24" s="19">
+      <c r="F24" s="17">
         <f>F51/B60*D60</f>
         <v>0.23444100000000001</v>
       </c>
@@ -2032,23 +2032,23 @@
       <c r="A25" s="5">
         <v>3</v>
       </c>
-      <c r="B25" s="19">
+      <c r="B25" s="17">
         <f>B52/B60*D60</f>
         <v>0.19810949999999999</v>
       </c>
-      <c r="C25" s="19">
+      <c r="C25" s="17">
         <f>C52/B60*D60</f>
         <v>0.21461862500000001</v>
       </c>
-      <c r="D25" s="19">
+      <c r="D25" s="17">
         <f>D52/B60*D60</f>
         <v>0.21461862500000001</v>
       </c>
-      <c r="E25" s="19">
+      <c r="E25" s="17">
         <f>E52/B60*D60</f>
         <v>0.21461862500000001</v>
       </c>
-      <c r="F25" s="19">
+      <c r="F25" s="17">
         <f>F52/B60*D60</f>
         <v>0.29339400000000004</v>
       </c>
@@ -2057,23 +2057,23 @@
       <c r="A26" s="5">
         <v>4</v>
       </c>
-      <c r="B26" s="19">
+      <c r="B26" s="17">
         <f>B53/B60*D60</f>
         <v>0.17914400000000003</v>
       </c>
-      <c r="C26" s="19">
+      <c r="C26" s="17">
         <f>C53/B60*D60</f>
         <v>0.382052</v>
       </c>
-      <c r="D26" s="19">
+      <c r="D26" s="17">
         <f>D53/B60*D60</f>
         <v>0.382052</v>
       </c>
-      <c r="E26" s="19">
+      <c r="E26" s="17">
         <f>E53/B60*D60</f>
         <v>0.382052</v>
       </c>
-      <c r="F26" s="19">
+      <c r="F26" s="17">
         <f>F53/B60*D60</f>
         <v>0.23764000000000002</v>
       </c>
@@ -2082,23 +2082,23 @@
       <c r="A27" s="5">
         <v>5</v>
       </c>
-      <c r="B27" s="19">
+      <c r="B27" s="17">
         <f>B54/B60*D60</f>
         <v>0.46979600000000005</v>
       </c>
-      <c r="C27" s="19">
+      <c r="C27" s="17">
         <f>C54/B60*D60</f>
         <v>0.23581200000000002</v>
       </c>
-      <c r="D27" s="19">
+      <c r="D27" s="17">
         <f>D54/B60*D60</f>
         <v>0.23581200000000002</v>
       </c>
-      <c r="E27" s="19">
+      <c r="E27" s="17">
         <f>E54/B60*D60</f>
         <v>0.23581200000000002</v>
       </c>
-      <c r="F27" s="19">
+      <c r="F27" s="17">
         <f>F54/B60*D60</f>
         <v>0.13213012500000001</v>
       </c>
@@ -2107,23 +2107,23 @@
       <c r="A28" s="5">
         <v>6</v>
       </c>
-      <c r="B28" s="19">
+      <c r="B28" s="17">
         <f>B55/B60*D60</f>
         <v>1.84228125E-2</v>
       </c>
-      <c r="C28" s="19">
+      <c r="C28" s="17">
         <f>C55/B60*D60</f>
         <v>1.84228125E-2</v>
       </c>
-      <c r="D28" s="19">
+      <c r="D28" s="17">
         <f>D55/B60*D60</f>
         <v>1.84228125E-2</v>
       </c>
-      <c r="E28" s="19">
+      <c r="E28" s="17">
         <f>E55/B60*D60</f>
         <v>8.1060375000000004E-2</v>
       </c>
-      <c r="F28" s="19">
+      <c r="F28" s="17">
         <f>F55/B60*D60</f>
         <v>0</v>
       </c>
@@ -2132,36 +2132,36 @@
       <c r="A29" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B29" s="19">
+      <c r="B29" s="17">
         <f>SUM(B23:B28)</f>
         <v>0.93402231250000012</v>
       </c>
-      <c r="C29" s="19">
+      <c r="C29" s="17">
         <f t="shared" ref="C29:F29" si="1">SUM(C23:C28)</f>
         <v>0.92356843749999995</v>
       </c>
-      <c r="D29" s="19">
+      <c r="D29" s="17">
         <f t="shared" si="1"/>
         <v>0.92356843749999995</v>
       </c>
-      <c r="E29" s="19">
+      <c r="E29" s="17">
         <f t="shared" si="1"/>
         <v>0.98620599999999992</v>
       </c>
-      <c r="F29" s="19">
+      <c r="F29" s="17">
         <f t="shared" si="1"/>
         <v>0.90514562500000006</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="11" t="s">
+      <c r="A31" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
@@ -2207,14 +2207,14 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="11" t="s">
+      <c r="A36" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B36" s="11"/>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
@@ -2240,19 +2240,19 @@
       <c r="A38" s="5">
         <v>1</v>
       </c>
-      <c r="B38" s="15">
+      <c r="B38" s="13">
         <v>160</v>
       </c>
-      <c r="C38" s="15">
+      <c r="C38" s="13">
         <v>448</v>
       </c>
-      <c r="D38" s="15">
+      <c r="D38" s="13">
         <v>448</v>
       </c>
-      <c r="E38" s="15">
+      <c r="E38" s="13">
         <v>448</v>
       </c>
-      <c r="F38" s="15">
+      <c r="F38" s="13">
         <v>528</v>
       </c>
     </row>
@@ -2260,19 +2260,19 @@
       <c r="A39" s="5">
         <v>2</v>
       </c>
-      <c r="B39" s="15">
+      <c r="B39" s="13">
         <v>4640</v>
       </c>
-      <c r="C39" s="15">
+      <c r="C39" s="13">
         <v>4640</v>
       </c>
-      <c r="D39" s="15">
+      <c r="D39" s="13">
         <v>4640</v>
       </c>
-      <c r="E39" s="15">
+      <c r="E39" s="13">
         <v>4640</v>
       </c>
-      <c r="F39" s="15">
+      <c r="F39" s="13">
         <v>16416</v>
       </c>
     </row>
@@ -2280,19 +2280,19 @@
       <c r="A40" s="5">
         <v>3</v>
       </c>
-      <c r="B40" s="15">
+      <c r="B40" s="13">
         <v>13872</v>
       </c>
-      <c r="C40" s="15">
+      <c r="C40" s="13">
         <v>15028</v>
       </c>
-      <c r="D40" s="15">
+      <c r="D40" s="13">
         <v>15028</v>
       </c>
-      <c r="E40" s="15">
+      <c r="E40" s="13">
         <v>15028</v>
       </c>
-      <c r="F40" s="15">
+      <c r="F40" s="13">
         <v>20544</v>
       </c>
     </row>
@@ -2300,19 +2300,19 @@
       <c r="A41" s="5">
         <v>4</v>
       </c>
-      <c r="B41" s="15">
+      <c r="B41" s="13">
         <v>12544</v>
       </c>
-      <c r="C41" s="15">
+      <c r="C41" s="13">
         <v>26752</v>
       </c>
-      <c r="D41" s="15">
+      <c r="D41" s="13">
         <v>26752</v>
       </c>
-      <c r="E41" s="15">
+      <c r="E41" s="13">
         <v>26752</v>
       </c>
-      <c r="F41" s="15">
+      <c r="F41" s="13">
         <v>16640</v>
       </c>
     </row>
@@ -2320,19 +2320,19 @@
       <c r="A42" s="5">
         <v>5</v>
       </c>
-      <c r="B42" s="15">
+      <c r="B42" s="13">
         <v>32896</v>
       </c>
-      <c r="C42" s="15">
+      <c r="C42" s="13">
         <v>16512</v>
       </c>
-      <c r="D42" s="15">
+      <c r="D42" s="13">
         <v>16512</v>
       </c>
-      <c r="E42" s="15">
+      <c r="E42" s="13">
         <v>16512</v>
       </c>
-      <c r="F42" s="15">
+      <c r="F42" s="13">
         <v>9252</v>
       </c>
     </row>
@@ -2340,19 +2340,19 @@
       <c r="A43" s="5">
         <v>6</v>
       </c>
-      <c r="B43" s="15">
+      <c r="B43" s="13">
         <v>1290</v>
       </c>
-      <c r="C43" s="15">
+      <c r="C43" s="13">
         <v>1290</v>
       </c>
-      <c r="D43" s="15">
+      <c r="D43" s="13">
         <v>1290</v>
       </c>
-      <c r="E43" s="15">
+      <c r="E43" s="13">
         <v>5676</v>
       </c>
-      <c r="F43" s="15">
+      <c r="F43" s="13">
         <v>0</v>
       </c>
     </row>
@@ -2360,23 +2360,23 @@
       <c r="A44" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B44" s="15">
+      <c r="B44" s="13">
         <f>SUM(B38:B43)</f>
         <v>65402</v>
       </c>
-      <c r="C44" s="15">
+      <c r="C44" s="13">
         <f t="shared" ref="C44:F44" si="2">SUM(C38:C43)</f>
         <v>64670</v>
       </c>
-      <c r="D44" s="15">
+      <c r="D44" s="13">
         <f t="shared" si="2"/>
         <v>64670</v>
       </c>
-      <c r="E44" s="15">
+      <c r="E44" s="13">
         <f t="shared" si="2"/>
         <v>69056</v>
       </c>
-      <c r="F44" s="15">
+      <c r="F44" s="13">
         <f t="shared" si="2"/>
         <v>63380</v>
       </c>
@@ -2385,46 +2385,46 @@
       <c r="A45" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B45" s="16">
+      <c r="B45" s="14">
         <f>B44*2/1000</f>
         <v>130.804</v>
       </c>
-      <c r="C45" s="16">
+      <c r="C45" s="14">
         <f t="shared" ref="C45:F45" si="3">C44*2/1000</f>
         <v>129.34</v>
       </c>
-      <c r="D45" s="16">
+      <c r="D45" s="14">
         <f t="shared" si="3"/>
         <v>129.34</v>
       </c>
-      <c r="E45" s="16">
+      <c r="E45" s="14">
         <f t="shared" si="3"/>
         <v>138.11199999999999</v>
       </c>
-      <c r="F45" s="16">
+      <c r="F45" s="14">
         <f t="shared" si="3"/>
         <v>126.76</v>
       </c>
     </row>
     <row r="46" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="18"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="18"/>
+      <c r="B46" s="16"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="16"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="16"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="9"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="11" t="s">
+      <c r="A48" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B48" s="11"/>
-      <c r="C48" s="11"/>
-      <c r="D48" s="11"/>
-      <c r="E48" s="11"/>
-      <c r="F48" s="11"/>
+      <c r="B48" s="18"/>
+      <c r="C48" s="18"/>
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
@@ -2450,23 +2450,23 @@
       <c r="A50" s="5">
         <v>1</v>
       </c>
-      <c r="B50" s="15">
+      <c r="B50" s="13">
         <f>B38*2/1000</f>
         <v>0.32</v>
       </c>
-      <c r="C50" s="15">
+      <c r="C50" s="13">
         <f t="shared" ref="C50:F50" si="4">C38*2/1000</f>
         <v>0.89600000000000002</v>
       </c>
-      <c r="D50" s="15">
+      <c r="D50" s="13">
         <f t="shared" si="4"/>
         <v>0.89600000000000002</v>
       </c>
-      <c r="E50" s="15">
+      <c r="E50" s="13">
         <f t="shared" si="4"/>
         <v>0.89600000000000002</v>
       </c>
-      <c r="F50" s="15">
+      <c r="F50" s="13">
         <f t="shared" si="4"/>
         <v>1.056</v>
       </c>
@@ -2475,23 +2475,23 @@
       <c r="A51" s="5">
         <v>2</v>
       </c>
-      <c r="B51" s="15">
+      <c r="B51" s="13">
         <f t="shared" ref="B51:F55" si="5">B39*2/1000</f>
         <v>9.2799999999999994</v>
       </c>
-      <c r="C51" s="15">
+      <c r="C51" s="13">
         <f t="shared" si="5"/>
         <v>9.2799999999999994</v>
       </c>
-      <c r="D51" s="15">
+      <c r="D51" s="13">
         <f t="shared" si="5"/>
         <v>9.2799999999999994</v>
       </c>
-      <c r="E51" s="15">
+      <c r="E51" s="13">
         <f t="shared" si="5"/>
         <v>9.2799999999999994</v>
       </c>
-      <c r="F51" s="15">
+      <c r="F51" s="13">
         <f t="shared" si="5"/>
         <v>32.832000000000001</v>
       </c>
@@ -2500,23 +2500,23 @@
       <c r="A52" s="5">
         <v>3</v>
       </c>
-      <c r="B52" s="15">
+      <c r="B52" s="13">
         <f t="shared" si="5"/>
         <v>27.744</v>
       </c>
-      <c r="C52" s="15">
+      <c r="C52" s="13">
         <f t="shared" si="5"/>
         <v>30.056000000000001</v>
       </c>
-      <c r="D52" s="15">
+      <c r="D52" s="13">
         <f t="shared" si="5"/>
         <v>30.056000000000001</v>
       </c>
-      <c r="E52" s="15">
+      <c r="E52" s="13">
         <f t="shared" si="5"/>
         <v>30.056000000000001</v>
       </c>
-      <c r="F52" s="15">
+      <c r="F52" s="13">
         <f t="shared" si="5"/>
         <v>41.088000000000001</v>
       </c>
@@ -2525,23 +2525,23 @@
       <c r="A53" s="5">
         <v>4</v>
       </c>
-      <c r="B53" s="15">
+      <c r="B53" s="13">
         <f t="shared" si="5"/>
         <v>25.088000000000001</v>
       </c>
-      <c r="C53" s="15">
+      <c r="C53" s="13">
         <f t="shared" si="5"/>
         <v>53.503999999999998</v>
       </c>
-      <c r="D53" s="15">
+      <c r="D53" s="13">
         <f t="shared" si="5"/>
         <v>53.503999999999998</v>
       </c>
-      <c r="E53" s="15">
+      <c r="E53" s="13">
         <f t="shared" si="5"/>
         <v>53.503999999999998</v>
       </c>
-      <c r="F53" s="15">
+      <c r="F53" s="13">
         <f t="shared" si="5"/>
         <v>33.28</v>
       </c>
@@ -2550,23 +2550,23 @@
       <c r="A54" s="5">
         <v>5</v>
       </c>
-      <c r="B54" s="15">
+      <c r="B54" s="13">
         <f t="shared" si="5"/>
         <v>65.792000000000002</v>
       </c>
-      <c r="C54" s="15">
+      <c r="C54" s="13">
         <f t="shared" si="5"/>
         <v>33.024000000000001</v>
       </c>
-      <c r="D54" s="15">
+      <c r="D54" s="13">
         <f t="shared" si="5"/>
         <v>33.024000000000001</v>
       </c>
-      <c r="E54" s="15">
+      <c r="E54" s="13">
         <f t="shared" si="5"/>
         <v>33.024000000000001</v>
       </c>
-      <c r="F54" s="15">
+      <c r="F54" s="13">
         <f t="shared" si="5"/>
         <v>18.504000000000001</v>
       </c>
@@ -2575,23 +2575,23 @@
       <c r="A55" s="5">
         <v>6</v>
       </c>
-      <c r="B55" s="15">
+      <c r="B55" s="13">
         <f t="shared" si="5"/>
         <v>2.58</v>
       </c>
-      <c r="C55" s="15">
+      <c r="C55" s="13">
         <f t="shared" si="5"/>
         <v>2.58</v>
       </c>
-      <c r="D55" s="15">
+      <c r="D55" s="13">
         <f t="shared" si="5"/>
         <v>2.58</v>
       </c>
-      <c r="E55" s="15">
+      <c r="E55" s="13">
         <f t="shared" si="5"/>
         <v>11.352</v>
       </c>
-      <c r="F55" s="15">
+      <c r="F55" s="13">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2600,41 +2600,41 @@
       <c r="A56" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B56" s="15">
+      <c r="B56" s="13">
         <f>SUM(B50:B55)</f>
         <v>130.804</v>
       </c>
-      <c r="C56" s="15">
+      <c r="C56" s="13">
         <f t="shared" ref="C56" si="6">SUM(C50:C55)</f>
         <v>129.34</v>
       </c>
-      <c r="D56" s="15">
+      <c r="D56" s="13">
         <f t="shared" ref="D56" si="7">SUM(D50:D55)</f>
         <v>129.34</v>
       </c>
-      <c r="E56" s="15">
+      <c r="E56" s="13">
         <f t="shared" ref="E56" si="8">SUM(E50:E55)</f>
         <v>138.11199999999999</v>
       </c>
-      <c r="F56" s="15">
+      <c r="F56" s="13">
         <f t="shared" ref="F56" si="9">SUM(F50:F55)</f>
         <v>126.76</v>
       </c>
     </row>
     <row r="57" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B57" s="17"/>
-      <c r="C57" s="17"/>
-      <c r="D57" s="17"/>
-      <c r="E57" s="17"/>
-      <c r="F57" s="17"/>
+      <c r="B57" s="15"/>
+      <c r="C57" s="15"/>
+      <c r="D57" s="15"/>
+      <c r="E57" s="15"/>
+      <c r="F57" s="15"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" s="11" t="s">
+      <c r="A59" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B59" s="11"/>
-      <c r="C59" s="11"/>
-      <c r="D59" s="11"/>
+      <c r="B59" s="18"/>
+      <c r="C59" s="18"/>
+      <c r="D59" s="18"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
@@ -2651,14 +2651,14 @@
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" s="11" t="s">
+      <c r="A63" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B63" s="11"/>
-      <c r="C63" s="11"/>
-      <c r="D63" s="11"/>
-      <c r="E63" s="11"/>
-      <c r="F63" s="11"/>
+      <c r="B63" s="18"/>
+      <c r="C63" s="18"/>
+      <c r="D63" s="18"/>
+      <c r="E63" s="18"/>
+      <c r="F63" s="18"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="1"/>
@@ -2725,14 +2725,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A63:F63"/>
+    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="A48:F48"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A11:F11"/>
     <mergeCell ref="A31:F31"/>
     <mergeCell ref="A36:F36"/>
     <mergeCell ref="A59:D59"/>
-    <mergeCell ref="A63:F63"/>
-    <mergeCell ref="A21:F21"/>
-    <mergeCell ref="A48:F48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>